<commit_message>
Just an updated UI Path code. Registering with C.R.U.D completly works now. Content collection is finished, but needs cleaning, finishing send off and report collection.
</commit_message>
<xml_diff>
--- a/Project UI Path/Assets/Clients.xlsx
+++ b/Project UI Path/Assets/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Work\QA Consulting\Training Notes\Project (5 - 9)\Project UI Path\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF70439-1C40-4ECD-9F6A-19AD03A22A86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D470B307-4626-4051-A0B9-7476D6D721B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{CE40C8E0-BA54-4B2C-812C-5A83F699B300}"/>
+    <workbookView xWindow="-22890" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{CE40C8E0-BA54-4B2C-812C-5A83F699B300}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -64,6 +64,36 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>62 West Wallaby Street</t>
+  </si>
+  <si>
+    <t>Wigan</t>
+  </si>
+  <si>
+    <t>W1 GAN</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>+44 07987 654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chris.lucas@qa.com </t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>DAILY​</t>
   </si>
 </sst>
 </file>
@@ -451,10 +481,13 @@
   <dimension ref="B2:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -492,7 +525,39 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J3" s="3"/>
+      <c r="B3">
+        <v>1592999959</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>